<commit_message>
New forms & updates
</commit_message>
<xml_diff>
--- a/ILRG_ORAM_I_encontros_drp/ILRG_ORAM_I_encontros_drp-media/ILRG_ORAM_I_encontros_drp.xlsx
+++ b/ILRG_ORAM_I_encontros_drp/ILRG_ORAM_I_encontros_drp-media/ILRG_ORAM_I_encontros_drp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\oram\ODK Forms\ILRG_ORAM_odk_forms\ILRG_ORAM_I_encontros_drp\ILRG_ORAM_I_encontros_drp-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FC3E71-6CA7-4A27-B5FC-F4A6D2F281CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254ACC59-7307-4C5A-BD2D-F520C7B87D00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -3728,9 +3728,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3961,395 +3968,396 @@
   </borders>
   <cellStyleXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="234" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="234" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="245" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="245" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="245" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="245" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="245" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="245" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="245" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="245"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="245" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="240" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="245" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="245" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="245"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="240" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="246">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5561,11 +5569,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6010,7 +6018,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="66" t="s">
         <v>1133</v>
       </c>
       <c r="B43" s="34" t="s">
@@ -31610,7 +31618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>